<commit_message>
Archivos de generacion de termicas por completar. Archivo de fuels por completar
</commit_message>
<xml_diff>
--- a/Oferta/Plantas renovables 2.xlsx
+++ b/Oferta/Plantas renovables 2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Switch UH\BDLP_nov 22\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicoquintero/Documents/Investigacion andes-EDF/Switch/Sin título/Oferta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F295A8BC-548C-44B5-B51A-C34871FF629C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7542FDB-80AE-DC40-91F4-8FA56138DE94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cgndco" sheetId="1" r:id="rId1"/>
@@ -1531,7 +1531,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2070,7 +2070,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2358,21 +2358,26 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L491"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="12" max="12" width="14.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2410,7 +2415,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2448,7 +2453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2486,7 +2491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2524,7 +2529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2562,7 +2567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2600,7 +2605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2638,7 +2643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2676,7 +2681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>9</v>
       </c>
@@ -2714,7 +2719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>10</v>
       </c>
@@ -2752,7 +2757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>13</v>
       </c>
@@ -2790,7 +2795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>14</v>
       </c>
@@ -2828,7 +2833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>15</v>
       </c>
@@ -2866,7 +2871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>16</v>
       </c>
@@ -2904,7 +2909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>17</v>
       </c>
@@ -2942,7 +2947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>18</v>
       </c>
@@ -2980,7 +2985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>19</v>
       </c>
@@ -3018,7 +3023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>20</v>
       </c>
@@ -3056,7 +3061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>21</v>
       </c>
@@ -3094,7 +3099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>22</v>
       </c>
@@ -3132,7 +3137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>23</v>
       </c>
@@ -3170,7 +3175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>24</v>
       </c>
@@ -3208,7 +3213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>25</v>
       </c>
@@ -3246,7 +3251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>28</v>
       </c>
@@ -3284,7 +3289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>29</v>
       </c>
@@ -3322,7 +3327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>30</v>
       </c>
@@ -3360,7 +3365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>31</v>
       </c>
@@ -3398,7 +3403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>32</v>
       </c>
@@ -3436,7 +3441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>34</v>
       </c>
@@ -3474,7 +3479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>35</v>
       </c>
@@ -3512,7 +3517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>40</v>
       </c>
@@ -3550,7 +3555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>41</v>
       </c>
@@ -3588,7 +3593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>42</v>
       </c>
@@ -3626,7 +3631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>45</v>
       </c>
@@ -3664,7 +3669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>50</v>
       </c>
@@ -3702,7 +3707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>51</v>
       </c>
@@ -3740,7 +3745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>53</v>
       </c>
@@ -3778,7 +3783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>54</v>
       </c>
@@ -3816,7 +3821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>56</v>
       </c>
@@ -3854,7 +3859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>57</v>
       </c>
@@ -3892,7 +3897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>58</v>
       </c>
@@ -3930,7 +3935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>60</v>
       </c>
@@ -3968,7 +3973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>61</v>
       </c>
@@ -4006,7 +4011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>62</v>
       </c>
@@ -4044,7 +4049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>63</v>
       </c>
@@ -4082,7 +4087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>64</v>
       </c>
@@ -4120,7 +4125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>65</v>
       </c>
@@ -4158,7 +4163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>67</v>
       </c>
@@ -4196,7 +4201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>69</v>
       </c>
@@ -4234,7 +4239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>70</v>
       </c>
@@ -4272,7 +4277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>71</v>
       </c>
@@ -4310,7 +4315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>73</v>
       </c>
@@ -4348,7 +4353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>74</v>
       </c>
@@ -4386,7 +4391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>75</v>
       </c>
@@ -4424,7 +4429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>76</v>
       </c>
@@ -4462,7 +4467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>77</v>
       </c>
@@ -4500,7 +4505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>78</v>
       </c>
@@ -4538,7 +4543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>79</v>
       </c>
@@ -4576,7 +4581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>81</v>
       </c>
@@ -4614,7 +4619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>82</v>
       </c>
@@ -4652,7 +4657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>83</v>
       </c>
@@ -4690,7 +4695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>84</v>
       </c>
@@ -4728,7 +4733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>86</v>
       </c>
@@ -4766,7 +4771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>87</v>
       </c>
@@ -4804,7 +4809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>88</v>
       </c>
@@ -4842,7 +4847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>89</v>
       </c>
@@ -4880,7 +4885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>90</v>
       </c>
@@ -4918,7 +4923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>91</v>
       </c>
@@ -4956,7 +4961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>92</v>
       </c>
@@ -4994,7 +4999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>93</v>
       </c>
@@ -5032,7 +5037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>94</v>
       </c>
@@ -5070,7 +5075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>95</v>
       </c>
@@ -5108,7 +5113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>96</v>
       </c>
@@ -5146,7 +5151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>97</v>
       </c>
@@ -5184,7 +5189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>98</v>
       </c>
@@ -5222,7 +5227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>99</v>
       </c>
@@ -5260,7 +5265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>100</v>
       </c>
@@ -5298,7 +5303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>101</v>
       </c>
@@ -5336,7 +5341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>103</v>
       </c>
@@ -5374,7 +5379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>104</v>
       </c>
@@ -5412,7 +5417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>105</v>
       </c>
@@ -5450,7 +5455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>106</v>
       </c>
@@ -5488,7 +5493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>107</v>
       </c>
@@ -5526,7 +5531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>108</v>
       </c>
@@ -5564,7 +5569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>109</v>
       </c>
@@ -5602,7 +5607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>110</v>
       </c>
@@ -5640,7 +5645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>112</v>
       </c>
@@ -5678,7 +5683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>113</v>
       </c>
@@ -5716,7 +5721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>114</v>
       </c>
@@ -5754,7 +5759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>115</v>
       </c>
@@ -5792,7 +5797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>122</v>
       </c>
@@ -5830,7 +5835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>126</v>
       </c>
@@ -5868,7 +5873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>127</v>
       </c>
@@ -5906,7 +5911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>128</v>
       </c>
@@ -5944,7 +5949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>130</v>
       </c>
@@ -5982,7 +5987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>131</v>
       </c>
@@ -6020,7 +6025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>132</v>
       </c>
@@ -6058,7 +6063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>133</v>
       </c>
@@ -6096,7 +6101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>134</v>
       </c>
@@ -6134,7 +6139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>135</v>
       </c>
@@ -6172,7 +6177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>136</v>
       </c>
@@ -6210,7 +6215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>137</v>
       </c>
@@ -6248,7 +6253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>138</v>
       </c>
@@ -6286,7 +6291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>139</v>
       </c>
@@ -6324,7 +6329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>140</v>
       </c>
@@ -6362,7 +6367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>141</v>
       </c>
@@ -6400,7 +6405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>142</v>
       </c>
@@ -6438,7 +6443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>143</v>
       </c>
@@ -6476,7 +6481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>144</v>
       </c>
@@ -6514,7 +6519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>145</v>
       </c>
@@ -6552,7 +6557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>146</v>
       </c>
@@ -6590,7 +6595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>147</v>
       </c>
@@ -6628,7 +6633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>148</v>
       </c>
@@ -6666,7 +6671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>149</v>
       </c>
@@ -6704,7 +6709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>150</v>
       </c>
@@ -6742,7 +6747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>151</v>
       </c>
@@ -6780,7 +6785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>153</v>
       </c>
@@ -6818,7 +6823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>154</v>
       </c>
@@ -6856,7 +6861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>155</v>
       </c>
@@ -6894,7 +6899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>156</v>
       </c>
@@ -6932,7 +6937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>157</v>
       </c>
@@ -6970,7 +6975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>158</v>
       </c>
@@ -7008,7 +7013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>159</v>
       </c>
@@ -7046,7 +7051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>160</v>
       </c>
@@ -7084,7 +7089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>161</v>
       </c>
@@ -7122,7 +7127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>162</v>
       </c>
@@ -7160,7 +7165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>163</v>
       </c>
@@ -7198,7 +7203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>164</v>
       </c>
@@ -7236,7 +7241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>165</v>
       </c>
@@ -7274,7 +7279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>166</v>
       </c>
@@ -7312,7 +7317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>167</v>
       </c>
@@ -7350,7 +7355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>172</v>
       </c>
@@ -7388,7 +7393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>174</v>
       </c>
@@ -7426,7 +7431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>177</v>
       </c>
@@ -7464,7 +7469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>178</v>
       </c>
@@ -7502,7 +7507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>179</v>
       </c>
@@ -7540,7 +7545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>180</v>
       </c>
@@ -7578,7 +7583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>181</v>
       </c>
@@ -7616,7 +7621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>182</v>
       </c>
@@ -7654,7 +7659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>183</v>
       </c>
@@ -7692,7 +7697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>184</v>
       </c>
@@ -7730,7 +7735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>185</v>
       </c>
@@ -7768,7 +7773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>186</v>
       </c>
@@ -7806,7 +7811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>187</v>
       </c>
@@ -7844,7 +7849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>188</v>
       </c>
@@ -7882,7 +7887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>189</v>
       </c>
@@ -7920,7 +7925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>190</v>
       </c>
@@ -7958,7 +7963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>191</v>
       </c>
@@ -7996,7 +8001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>192</v>
       </c>
@@ -8034,7 +8039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>193</v>
       </c>
@@ -8072,7 +8077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>194</v>
       </c>
@@ -8110,7 +8115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>195</v>
       </c>
@@ -8148,7 +8153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>196</v>
       </c>
@@ -8186,7 +8191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>198</v>
       </c>
@@ -8224,7 +8229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>199</v>
       </c>
@@ -8262,7 +8267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>200</v>
       </c>
@@ -8300,7 +8305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>201</v>
       </c>
@@ -8338,7 +8343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>202</v>
       </c>
@@ -8376,7 +8381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>203</v>
       </c>
@@ -8414,7 +8419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>204</v>
       </c>
@@ -8452,7 +8457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>205</v>
       </c>
@@ -8490,7 +8495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>206</v>
       </c>
@@ -8528,7 +8533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>207</v>
       </c>
@@ -8566,7 +8571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>208</v>
       </c>
@@ -8604,7 +8609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>209</v>
       </c>
@@ -8642,7 +8647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>210</v>
       </c>
@@ -8680,7 +8685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>211</v>
       </c>
@@ -8718,7 +8723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>212</v>
       </c>
@@ -8756,7 +8761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>213</v>
       </c>
@@ -8794,7 +8799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>214</v>
       </c>
@@ -8832,7 +8837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A171">
         <v>215</v>
       </c>
@@ -8870,7 +8875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>217</v>
       </c>
@@ -8908,7 +8913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A173">
         <v>218</v>
       </c>
@@ -8946,7 +8951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A174">
         <v>219</v>
       </c>
@@ -8984,7 +8989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A175">
         <v>220</v>
       </c>
@@ -9022,7 +9027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A176">
         <v>221</v>
       </c>
@@ -9060,7 +9065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>222</v>
       </c>
@@ -9098,7 +9103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>223</v>
       </c>
@@ -9136,7 +9141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>224</v>
       </c>
@@ -9174,7 +9179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>225</v>
       </c>
@@ -9212,7 +9217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>226</v>
       </c>
@@ -9250,7 +9255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>227</v>
       </c>
@@ -9288,7 +9293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A183">
         <v>229</v>
       </c>
@@ -9326,7 +9331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>230</v>
       </c>
@@ -9364,7 +9369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A185">
         <v>231</v>
       </c>
@@ -9402,7 +9407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>232</v>
       </c>
@@ -9440,7 +9445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>233</v>
       </c>
@@ -9478,7 +9483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A188">
         <v>234</v>
       </c>
@@ -9516,7 +9521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A189">
         <v>235</v>
       </c>
@@ -9554,7 +9559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>236</v>
       </c>
@@ -9592,7 +9597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A191">
         <v>237</v>
       </c>
@@ -9630,7 +9635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A192">
         <v>238</v>
       </c>
@@ -9668,7 +9673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A193">
         <v>239</v>
       </c>
@@ -9706,7 +9711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A194">
         <v>240</v>
       </c>
@@ -9744,7 +9749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A195">
         <v>241</v>
       </c>
@@ -9782,7 +9787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A196">
         <v>242</v>
       </c>
@@ -9820,7 +9825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A197">
         <v>243</v>
       </c>
@@ -9858,7 +9863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A198">
         <v>244</v>
       </c>
@@ -9896,7 +9901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A199">
         <v>245</v>
       </c>
@@ -9934,7 +9939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A200">
         <v>246</v>
       </c>
@@ -9972,7 +9977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A201">
         <v>247</v>
       </c>
@@ -10010,7 +10015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A202">
         <v>248</v>
       </c>
@@ -10048,7 +10053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A203">
         <v>249</v>
       </c>
@@ -10086,7 +10091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A204">
         <v>250</v>
       </c>
@@ -10124,7 +10129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A205">
         <v>251</v>
       </c>
@@ -10162,7 +10167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A206">
         <v>252</v>
       </c>
@@ -10200,7 +10205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A207">
         <v>253</v>
       </c>
@@ -10238,7 +10243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A208">
         <v>254</v>
       </c>
@@ -10276,7 +10281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A209">
         <v>255</v>
       </c>
@@ -10314,7 +10319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A210">
         <v>256</v>
       </c>
@@ -10352,7 +10357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A211">
         <v>257</v>
       </c>
@@ -10390,7 +10395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A212">
         <v>258</v>
       </c>
@@ -10428,7 +10433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A213">
         <v>259</v>
       </c>
@@ -10466,7 +10471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A214">
         <v>260</v>
       </c>
@@ -10504,7 +10509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A215">
         <v>261</v>
       </c>
@@ -10542,7 +10547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A216">
         <v>262</v>
       </c>
@@ -10580,7 +10585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A217">
         <v>263</v>
       </c>
@@ -10618,7 +10623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A218">
         <v>264</v>
       </c>
@@ -10656,7 +10661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A219">
         <v>265</v>
       </c>
@@ -10694,7 +10699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A220">
         <v>266</v>
       </c>
@@ -10732,7 +10737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A221">
         <v>267</v>
       </c>
@@ -10770,7 +10775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A222">
         <v>268</v>
       </c>
@@ -10808,7 +10813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A223">
         <v>269</v>
       </c>
@@ -10846,7 +10851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A224">
         <v>270</v>
       </c>
@@ -10884,7 +10889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A225">
         <v>271</v>
       </c>
@@ -10922,7 +10927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A226">
         <v>272</v>
       </c>
@@ -10960,7 +10965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A227">
         <v>273</v>
       </c>
@@ -10998,7 +11003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A228">
         <v>274</v>
       </c>
@@ -11036,7 +11041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A229">
         <v>276</v>
       </c>
@@ -11074,7 +11079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A230">
         <v>277</v>
       </c>
@@ -11112,7 +11117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A231">
         <v>278</v>
       </c>
@@ -11150,7 +11155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A232">
         <v>279</v>
       </c>
@@ -11188,7 +11193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A233">
         <v>280</v>
       </c>
@@ -11226,7 +11231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A234">
         <v>281</v>
       </c>
@@ -11264,7 +11269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A235">
         <v>282</v>
       </c>
@@ -11302,7 +11307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A236">
         <v>283</v>
       </c>
@@ -11340,7 +11345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A237">
         <v>284</v>
       </c>
@@ -11378,7 +11383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A238">
         <v>285</v>
       </c>
@@ -11416,7 +11421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A239">
         <v>286</v>
       </c>
@@ -11454,7 +11459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A240">
         <v>287</v>
       </c>
@@ -11492,7 +11497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A241">
         <v>288</v>
       </c>
@@ -11530,7 +11535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A242">
         <v>289</v>
       </c>
@@ -11568,7 +11573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A243">
         <v>290</v>
       </c>
@@ -11606,7 +11611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A244">
         <v>291</v>
       </c>
@@ -11644,7 +11649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A245">
         <v>292</v>
       </c>
@@ -11682,7 +11687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A246">
         <v>293</v>
       </c>
@@ -11720,7 +11725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A247">
         <v>294</v>
       </c>
@@ -11758,7 +11763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A248">
         <v>295</v>
       </c>
@@ -11796,7 +11801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A249">
         <v>297</v>
       </c>
@@ -11834,7 +11839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A250">
         <v>298</v>
       </c>
@@ -11872,7 +11877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A251">
         <v>299</v>
       </c>
@@ -11910,7 +11915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A252">
         <v>300</v>
       </c>
@@ -11948,7 +11953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A253">
         <v>301</v>
       </c>
@@ -11986,7 +11991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A254">
         <v>302</v>
       </c>
@@ -12024,7 +12029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A255">
         <v>303</v>
       </c>
@@ -12062,7 +12067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A256">
         <v>304</v>
       </c>
@@ -12100,7 +12105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A257">
         <v>305</v>
       </c>
@@ -12138,7 +12143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A258">
         <v>306</v>
       </c>
@@ -12176,7 +12181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A259">
         <v>307</v>
       </c>
@@ -12214,7 +12219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A260">
         <v>308</v>
       </c>
@@ -12252,7 +12257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A261">
         <v>309</v>
       </c>
@@ -12290,7 +12295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A262">
         <v>310</v>
       </c>
@@ -12328,7 +12333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A263">
         <v>311</v>
       </c>
@@ -12366,7 +12371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="264" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A264">
         <v>312</v>
       </c>
@@ -12404,7 +12409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A265">
         <v>313</v>
       </c>
@@ -12442,7 +12447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A266">
         <v>314</v>
       </c>
@@ -12480,7 +12485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A267">
         <v>315</v>
       </c>
@@ -12518,7 +12523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A268">
         <v>316</v>
       </c>
@@ -12556,7 +12561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A269">
         <v>317</v>
       </c>
@@ -12594,7 +12599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A270">
         <v>318</v>
       </c>
@@ -12632,7 +12637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A271">
         <v>319</v>
       </c>
@@ -12670,7 +12675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A272">
         <v>320</v>
       </c>
@@ -12708,7 +12713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A273">
         <v>321</v>
       </c>
@@ -12746,7 +12751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="274" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A274">
         <v>322</v>
       </c>
@@ -12784,7 +12789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="275" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A275">
         <v>323</v>
       </c>
@@ -12822,7 +12827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="276" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A276">
         <v>324</v>
       </c>
@@ -12860,7 +12865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="277" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A277">
         <v>325</v>
       </c>
@@ -12898,7 +12903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="278" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A278">
         <v>326</v>
       </c>
@@ -12936,7 +12941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="279" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A279">
         <v>327</v>
       </c>
@@ -12974,7 +12979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="280" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A280">
         <v>328</v>
       </c>
@@ -13012,7 +13017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="281" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A281">
         <v>329</v>
       </c>
@@ -13050,7 +13055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="282" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A282">
         <v>330</v>
       </c>
@@ -13088,7 +13093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="283" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A283">
         <v>331</v>
       </c>
@@ -13126,7 +13131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="284" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A284">
         <v>332</v>
       </c>
@@ -13164,7 +13169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="285" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A285">
         <v>333</v>
       </c>
@@ -13202,7 +13207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="286" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A286">
         <v>334</v>
       </c>
@@ -13240,7 +13245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="287" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A287">
         <v>335</v>
       </c>
@@ -13278,7 +13283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="288" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A288">
         <v>336</v>
       </c>
@@ -13316,7 +13321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="289" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A289">
         <v>337</v>
       </c>
@@ -13354,7 +13359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="290" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A290">
         <v>338</v>
       </c>
@@ -13392,7 +13397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="291" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A291">
         <v>339</v>
       </c>
@@ -13430,7 +13435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="292" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A292">
         <v>340</v>
       </c>
@@ -13468,7 +13473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="293" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A293">
         <v>341</v>
       </c>
@@ -13506,7 +13511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="294" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A294">
         <v>342</v>
       </c>
@@ -13544,7 +13549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="295" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A295">
         <v>343</v>
       </c>
@@ -13582,7 +13587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="296" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A296">
         <v>344</v>
       </c>
@@ -13620,7 +13625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="297" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A297">
         <v>345</v>
       </c>
@@ -13658,7 +13663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="298" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A298">
         <v>346</v>
       </c>
@@ -13696,7 +13701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="299" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A299">
         <v>347</v>
       </c>
@@ -13734,7 +13739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="300" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A300">
         <v>348</v>
       </c>
@@ -13772,7 +13777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="301" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A301">
         <v>349</v>
       </c>
@@ -13810,7 +13815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="302" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A302">
         <v>350</v>
       </c>
@@ -13848,7 +13853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="303" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A303">
         <v>351</v>
       </c>
@@ -13886,7 +13891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="304" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A304">
         <v>352</v>
       </c>
@@ -13924,7 +13929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="305" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A305">
         <v>353</v>
       </c>
@@ -13962,7 +13967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="306" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A306">
         <v>354</v>
       </c>
@@ -14000,7 +14005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="307" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A307">
         <v>355</v>
       </c>
@@ -14038,7 +14043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="308" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A308">
         <v>356</v>
       </c>
@@ -14076,7 +14081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="309" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A309">
         <v>357</v>
       </c>
@@ -14114,7 +14119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="310" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A310">
         <v>358</v>
       </c>
@@ -14152,7 +14157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="311" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A311">
         <v>359</v>
       </c>
@@ -14190,7 +14195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="312" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A312">
         <v>360</v>
       </c>
@@ -14228,7 +14233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="313" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A313">
         <v>361</v>
       </c>
@@ -14266,7 +14271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="314" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A314">
         <v>362</v>
       </c>
@@ -14304,7 +14309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="315" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A315">
         <v>363</v>
       </c>
@@ -14342,7 +14347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="316" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A316">
         <v>364</v>
       </c>
@@ -14380,7 +14385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="317" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A317">
         <v>365</v>
       </c>
@@ -14418,7 +14423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="318" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A318">
         <v>366</v>
       </c>
@@ -14456,7 +14461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="319" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A319">
         <v>367</v>
       </c>
@@ -14494,7 +14499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="320" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A320">
         <v>368</v>
       </c>
@@ -14532,7 +14537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="321" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A321">
         <v>369</v>
       </c>
@@ -14570,7 +14575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="322" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A322">
         <v>370</v>
       </c>
@@ -14608,7 +14613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="323" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A323">
         <v>371</v>
       </c>
@@ -14646,7 +14651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="324" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A324">
         <v>372</v>
       </c>
@@ -14684,7 +14689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="325" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A325">
         <v>373</v>
       </c>
@@ -14722,7 +14727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="326" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A326">
         <v>374</v>
       </c>
@@ -14760,7 +14765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="327" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A327">
         <v>375</v>
       </c>
@@ -14798,7 +14803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="328" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A328">
         <v>376</v>
       </c>
@@ -14836,7 +14841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="329" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A329">
         <v>377</v>
       </c>
@@ -14874,7 +14879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="330" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A330">
         <v>378</v>
       </c>
@@ -14912,7 +14917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="331" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A331">
         <v>379</v>
       </c>
@@ -14950,7 +14955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="332" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A332">
         <v>380</v>
       </c>
@@ -14988,7 +14993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="333" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A333">
         <v>381</v>
       </c>
@@ -15026,7 +15031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="334" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A334">
         <v>382</v>
       </c>
@@ -15064,7 +15069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="335" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A335">
         <v>383</v>
       </c>
@@ -15102,7 +15107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="336" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A336">
         <v>384</v>
       </c>
@@ -15140,7 +15145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="337" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A337">
         <v>385</v>
       </c>
@@ -15178,7 +15183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="338" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A338">
         <v>386</v>
       </c>
@@ -15216,7 +15221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="339" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A339">
         <v>387</v>
       </c>
@@ -15254,7 +15259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="340" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A340">
         <v>388</v>
       </c>
@@ -15292,7 +15297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="341" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A341">
         <v>389</v>
       </c>
@@ -15330,7 +15335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="342" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A342">
         <v>390</v>
       </c>
@@ -15368,7 +15373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="343" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A343">
         <v>391</v>
       </c>
@@ -15406,7 +15411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="344" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A344">
         <v>392</v>
       </c>
@@ -15444,7 +15449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="345" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A345">
         <v>393</v>
       </c>
@@ -15482,7 +15487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="346" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A346">
         <v>394</v>
       </c>
@@ -15520,7 +15525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="347" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A347">
         <v>395</v>
       </c>
@@ -15558,7 +15563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="348" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A348">
         <v>396</v>
       </c>
@@ -15596,7 +15601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="349" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A349">
         <v>397</v>
       </c>
@@ -15634,7 +15639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="350" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A350">
         <v>398</v>
       </c>
@@ -15672,7 +15677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="351" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A351">
         <v>399</v>
       </c>
@@ -15710,7 +15715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="352" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A352">
         <v>400</v>
       </c>
@@ -15748,7 +15753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="353" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A353">
         <v>401</v>
       </c>
@@ -15786,7 +15791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="354" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A354">
         <v>402</v>
       </c>
@@ -15824,7 +15829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="355" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A355">
         <v>403</v>
       </c>
@@ -15862,7 +15867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="356" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A356">
         <v>404</v>
       </c>
@@ -15900,7 +15905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="357" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A357">
         <v>405</v>
       </c>
@@ -15938,7 +15943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="358" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A358">
         <v>406</v>
       </c>
@@ -15976,7 +15981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="359" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A359">
         <v>409</v>
       </c>
@@ -16014,7 +16019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="360" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A360">
         <v>410</v>
       </c>
@@ -16052,7 +16057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="361" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A361">
         <v>411</v>
       </c>
@@ -16090,7 +16095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="362" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A362">
         <v>412</v>
       </c>
@@ -16128,7 +16133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="363" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A363">
         <v>413</v>
       </c>
@@ -16166,7 +16171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="364" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A364">
         <v>414</v>
       </c>
@@ -16204,7 +16209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="365" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A365">
         <v>415</v>
       </c>
@@ -16242,7 +16247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="366" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A366">
         <v>416</v>
       </c>
@@ -16280,7 +16285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="367" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A367">
         <v>417</v>
       </c>
@@ -16318,7 +16323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="368" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A368">
         <v>418</v>
       </c>
@@ -16356,7 +16361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="369" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A369">
         <v>419</v>
       </c>
@@ -16394,7 +16399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="370" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A370">
         <v>420</v>
       </c>
@@ -16432,7 +16437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="371" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A371">
         <v>421</v>
       </c>
@@ -16470,7 +16475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="372" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A372">
         <v>422</v>
       </c>
@@ -16508,7 +16513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="373" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A373">
         <v>423</v>
       </c>
@@ -16546,7 +16551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="374" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A374">
         <v>407</v>
       </c>
@@ -16584,7 +16589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="375" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A375">
         <v>408</v>
       </c>
@@ -16622,7 +16627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="376" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A376">
         <v>424</v>
       </c>
@@ -16660,7 +16665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="377" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A377">
         <v>425</v>
       </c>
@@ -16698,7 +16703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="378" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A378">
         <v>426</v>
       </c>
@@ -16736,7 +16741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="379" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A379">
         <v>427</v>
       </c>
@@ -16774,7 +16779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="380" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A380">
         <v>428</v>
       </c>
@@ -16812,7 +16817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="381" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A381">
         <v>429</v>
       </c>
@@ -16850,7 +16855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="382" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A382">
         <v>430</v>
       </c>
@@ -16888,7 +16893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="383" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A383">
         <v>431</v>
       </c>
@@ -16926,7 +16931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="384" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A384">
         <v>432</v>
       </c>
@@ -16964,7 +16969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="385" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A385">
         <v>433</v>
       </c>
@@ -17002,7 +17007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="386" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A386">
         <v>434</v>
       </c>
@@ -17040,7 +17045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="387" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A387">
         <v>435</v>
       </c>
@@ -17078,7 +17083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="388" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A388">
         <v>436</v>
       </c>
@@ -17116,7 +17121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="389" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A389">
         <v>437</v>
       </c>
@@ -17154,7 +17159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="390" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A390">
         <v>438</v>
       </c>
@@ -17192,7 +17197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="391" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A391">
         <v>439</v>
       </c>
@@ -17230,7 +17235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="392" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A392">
         <v>440</v>
       </c>
@@ -17268,7 +17273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="393" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A393">
         <v>441</v>
       </c>
@@ -17306,7 +17311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="394" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A394">
         <v>442</v>
       </c>
@@ -17344,7 +17349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="395" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A395">
         <v>443</v>
       </c>
@@ -17382,7 +17387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="396" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A396">
         <v>444</v>
       </c>
@@ -17420,7 +17425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="397" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A397">
         <v>445</v>
       </c>
@@ -17458,7 +17463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="398" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A398">
         <v>446</v>
       </c>
@@ -17496,7 +17501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="399" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A399">
         <v>447</v>
       </c>
@@ -17534,7 +17539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="400" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A400">
         <v>448</v>
       </c>
@@ -17572,7 +17577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="401" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A401">
         <v>449</v>
       </c>
@@ -17610,7 +17615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="402" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A402">
         <v>450</v>
       </c>
@@ -17648,7 +17653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="403" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A403">
         <v>451</v>
       </c>
@@ -17686,7 +17691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="404" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A404">
         <v>452</v>
       </c>
@@ -17724,7 +17729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="405" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A405">
         <v>453</v>
       </c>
@@ -17762,7 +17767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="406" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A406">
         <v>454</v>
       </c>
@@ -17800,7 +17805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="407" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A407">
         <v>455</v>
       </c>
@@ -17838,7 +17843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="408" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A408">
         <v>456</v>
       </c>
@@ -17876,7 +17881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="409" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A409">
         <v>457</v>
       </c>
@@ -17914,7 +17919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="410" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A410">
         <v>458</v>
       </c>
@@ -17952,7 +17957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="411" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A411">
         <v>459</v>
       </c>
@@ -17990,7 +17995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="412" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A412">
         <v>460</v>
       </c>
@@ -18028,7 +18033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="413" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="413" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A413">
         <v>461</v>
       </c>
@@ -18066,7 +18071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="414" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="414" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A414">
         <v>462</v>
       </c>
@@ -18104,7 +18109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="415" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="415" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A415">
         <v>463</v>
       </c>
@@ -18142,7 +18147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="416" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="416" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A416">
         <v>464</v>
       </c>
@@ -18180,7 +18185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="417" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="417" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A417">
         <v>465</v>
       </c>
@@ -18218,7 +18223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="418" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="418" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A418">
         <v>466</v>
       </c>
@@ -18256,7 +18261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="419" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="419" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A419">
         <v>467</v>
       </c>
@@ -18294,7 +18299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="420" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="420" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A420">
         <v>468</v>
       </c>
@@ -18332,7 +18337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="421" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="421" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A421">
         <v>469</v>
       </c>
@@ -18370,7 +18375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="422" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="422" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A422">
         <v>470</v>
       </c>
@@ -18408,7 +18413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="423" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="423" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A423">
         <v>471</v>
       </c>
@@ -18446,7 +18451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="424" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="424" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A424">
         <v>472</v>
       </c>
@@ -18484,7 +18489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="425" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="425" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A425">
         <v>473</v>
       </c>
@@ -18522,7 +18527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="426" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="426" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A426">
         <v>474</v>
       </c>
@@ -18560,7 +18565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="427" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="427" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A427">
         <v>475</v>
       </c>
@@ -18598,7 +18603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="428" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="428" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A428">
         <v>476</v>
       </c>
@@ -18636,7 +18641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="429" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="429" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A429">
         <v>477</v>
       </c>
@@ -18674,7 +18679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="430" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="430" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A430">
         <v>478</v>
       </c>
@@ -18712,7 +18717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="431" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="431" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A431">
         <v>479</v>
       </c>
@@ -18750,7 +18755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="432" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="432" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A432">
         <v>480</v>
       </c>
@@ -18788,7 +18793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="433" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="433" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A433">
         <v>481</v>
       </c>
@@ -18826,7 +18831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="434" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="434" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A434">
         <v>482</v>
       </c>
@@ -18864,7 +18869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="435" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="435" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A435">
         <v>483</v>
       </c>
@@ -18902,7 +18907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="436" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="436" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A436">
         <v>484</v>
       </c>
@@ -18940,7 +18945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="437" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="437" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A437">
         <v>485</v>
       </c>
@@ -18978,7 +18983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="438" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="438" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A438">
         <v>486</v>
       </c>
@@ -19016,7 +19021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="439" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="439" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A439">
         <v>487</v>
       </c>
@@ -19054,7 +19059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="440" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="440" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A440">
         <v>488</v>
       </c>
@@ -19092,7 +19097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="441" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="441" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A441">
         <v>489</v>
       </c>
@@ -19130,7 +19135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="442" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="442" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A442">
         <v>490</v>
       </c>
@@ -19168,7 +19173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="443" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="443" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A443">
         <v>491</v>
       </c>
@@ -19206,7 +19211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="444" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="444" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A444">
         <v>492</v>
       </c>
@@ -19244,7 +19249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="445" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="445" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A445">
         <v>493</v>
       </c>
@@ -19282,7 +19287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="446" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="446" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A446">
         <v>494</v>
       </c>
@@ -19320,7 +19325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="447" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="447" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A447">
         <v>495</v>
       </c>
@@ -19358,7 +19363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="448" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="448" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A448">
         <v>496</v>
       </c>
@@ -19396,7 +19401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="449" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="449" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A449">
         <v>497</v>
       </c>
@@ -19434,7 +19439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="450" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="450" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A450">
         <v>498</v>
       </c>
@@ -19472,7 +19477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="451" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="451" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A451">
         <v>499</v>
       </c>
@@ -19510,7 +19515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="452" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="452" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A452">
         <v>500</v>
       </c>
@@ -19548,7 +19553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="453" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="453" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A453">
         <v>501</v>
       </c>
@@ -19586,7 +19591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="454" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="454" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A454">
         <v>502</v>
       </c>
@@ -19624,7 +19629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="455" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="455" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A455">
         <v>503</v>
       </c>
@@ -19662,7 +19667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="456" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="456" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A456">
         <v>504</v>
       </c>
@@ -19700,7 +19705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="457" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="457" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A457">
         <v>505</v>
       </c>
@@ -19738,7 +19743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="458" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="458" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A458">
         <v>506</v>
       </c>
@@ -19776,7 +19781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="459" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="459" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A459">
         <v>507</v>
       </c>
@@ -19814,7 +19819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="460" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="460" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A460">
         <v>508</v>
       </c>
@@ -19852,7 +19857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="461" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="461" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A461">
         <v>509</v>
       </c>
@@ -19890,7 +19895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="462" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="462" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A462">
         <v>510</v>
       </c>
@@ -19928,7 +19933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="463" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="463" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A463">
         <v>511</v>
       </c>
@@ -19966,7 +19971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="464" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="464" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A464">
         <v>512</v>
       </c>
@@ -20004,7 +20009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="465" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="465" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A465">
         <v>513</v>
       </c>
@@ -20042,7 +20047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="466" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="466" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A466">
         <v>514</v>
       </c>
@@ -20080,7 +20085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="467" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="467" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A467">
         <v>515</v>
       </c>
@@ -20118,7 +20123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="468" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="468" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A468">
         <v>516</v>
       </c>
@@ -20156,7 +20161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="469" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="469" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A469">
         <v>517</v>
       </c>
@@ -20194,7 +20199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="470" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="470" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A470">
         <v>518</v>
       </c>
@@ -20232,7 +20237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="471" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="471" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A471">
         <v>519</v>
       </c>
@@ -20270,7 +20275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="472" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="472" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A472">
         <v>520</v>
       </c>
@@ -20308,7 +20313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="473" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="473" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A473">
         <v>521</v>
       </c>
@@ -20346,7 +20351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="474" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="474" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A474">
         <v>522</v>
       </c>
@@ -20384,7 +20389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="475" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="475" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A475">
         <v>523</v>
       </c>
@@ -20422,7 +20427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="476" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="476" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A476">
         <v>524</v>
       </c>
@@ -20460,7 +20465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="477" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="477" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A477">
         <v>525</v>
       </c>
@@ -20498,7 +20503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="478" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="478" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A478">
         <v>526</v>
       </c>
@@ -20536,7 +20541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="479" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="479" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A479">
         <v>527</v>
       </c>
@@ -20574,7 +20579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="480" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="480" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A480">
         <v>528</v>
       </c>
@@ -20612,7 +20617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="481" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="481" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A481">
         <v>529</v>
       </c>
@@ -20650,7 +20655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="482" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="482" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A482">
         <v>530</v>
       </c>
@@ -20688,7 +20693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="483" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="483" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A483">
         <v>531</v>
       </c>
@@ -20726,7 +20731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="484" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="484" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A484">
         <v>532</v>
       </c>
@@ -20764,7 +20769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="485" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="485" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A485">
         <v>533</v>
       </c>
@@ -20802,7 +20807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="486" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="486" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A486">
         <v>534</v>
       </c>
@@ -20840,7 +20845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="487" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="487" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A487">
         <v>535</v>
       </c>
@@ -20878,7 +20883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="488" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="488" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A488">
         <v>536</v>
       </c>
@@ -20916,7 +20921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="489" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="489" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A489">
         <v>537</v>
       </c>
@@ -20954,7 +20959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="490" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="490" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A490">
         <v>538</v>
       </c>
@@ -20992,7 +20997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="491" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="491" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A491">
         <v>539</v>
       </c>
@@ -21036,6 +21041,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100A4C92F77D51DB34BB66DB547BA261888" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="036d0ed6745d5cb6fc93e88a90c24f29">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3901be2b-e0aa-425f-8ecd-05b022f3c304" xmlns:ns3="1d72c402-e5ab-4c37-8652-a8939ba1b122" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b8e2230f21ddac050465166b7244a911" ns2:_="" ns3:_="">
     <xsd:import namespace="3901be2b-e0aa-425f-8ecd-05b022f3c304"/>
@@ -21200,15 +21214,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -21216,13 +21221,37 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B727F1AF-3666-4AD2-B66C-A4438299235C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C27F50B0-445B-4E5D-8CA7-8E60627FF45A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C27F50B0-445B-4E5D-8CA7-8E60627FF45A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B727F1AF-3666-4AD2-B66C-A4438299235C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3901be2b-e0aa-425f-8ecd-05b022f3c304"/>
+    <ds:schemaRef ds:uri="1d72c402-e5ab-4c37-8652-a8939ba1b122"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C35AB643-3CC6-4CF0-97E8-A9D78E88D513}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C35AB643-3CC6-4CF0-97E8-A9D78E88D513}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>